<commit_message>
210521_cart, order 테이블 합치기
</commit_message>
<xml_diff>
--- a/스프링작업자료/Mapper/mapper기능정리.xlsx
+++ b/스프링작업자료/Mapper/mapper기능정리.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="405">
   <si>
     <t>default sysdate</t>
   </si>
@@ -1418,38 +1418,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>email, prodnum, quantity 검색 -&gt; 장바구니 안거치고 오더 테이블 삽입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result = 4 (바로구매 시) 최소하면 order 초기화 시 삭제 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 이름, 이미지 값 가져와서 삽입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>order_now</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>바로 구매 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>order_nowdelete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email, result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email, result(4) 검색 -&gt; 데이터 삭제 -&gt; 구매창 취소 시 사용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>defalut 1(배송전 : 1, 배송중 : 2, 배송완료:3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1491,6 +1463,65 @@
   </si>
   <si>
     <t>2@a.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니완료삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cart_redelete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니합계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cart_tot</t>
+  </si>
+  <si>
+    <t>cartnum, result(3 이하) 검색 -&gt; 합계 반환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum, result(3) 검색 -&gt; 해당 상품 삭제 -&gt; 장바구니 창 열때 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 품목 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum검색 -&gt; result(1) 수정 -&gt; 장바구니에는 존재함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_tot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cartnum, result(2) 검색 -&gt; 합계 반환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구메페이지합계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, prodnum, quantity 검색 -&gt; result(2)로 삽입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2254,8 +2285,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -2882,6 +2913,24 @@
         <v>101</v>
       </c>
       <c r="E22" s="3"/>
+      <c r="G22" s="19">
+        <v>7</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
@@ -2899,15 +2948,23 @@
       <c r="E23" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>290</v>
+      <c r="G23" s="19">
+        <v>8</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2924,23 +2981,23 @@
         <v>101</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="G24" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>127</v>
+      <c r="G24" s="21">
+        <v>9</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2957,23 +3014,23 @@
       <c r="E25" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="G25" s="21">
-        <v>1</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>368</v>
+      <c r="G25" s="19">
+        <v>10</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>398</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>367</v>
+        <v>136</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2988,13 +3045,23 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
+      <c r="G26" s="19">
+        <v>11</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>153</v>
+      </c>
       <c r="L26" s="13" t="s">
-        <v>369</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -3011,23 +3078,23 @@
       <c r="E27" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="G27" s="21">
-        <v>2</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>363</v>
+      <c r="G27" s="19">
+        <v>12</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>377</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>371</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3043,327 +3110,356 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="G28" s="19">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>372</v>
+        <v>402</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>259</v>
+        <v>400</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K28" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>136</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="G29" s="19">
-        <v>3</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="K29" s="15" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G32" s="18">
+        <v>1</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L29" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="G30" s="9">
-        <v>4</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="18">
-        <v>5</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>377</v>
-      </c>
-      <c r="K31" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31" t="s">
-        <v>379</v>
+      <c r="L32" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13" t="s">
-        <v>380</v>
+      <c r="E33" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="G34" s="18">
-        <v>5</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="K34" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>385</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="G35" s="18">
-        <v>6</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>185</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>335</v>
+      <c r="E36" s="3"/>
+      <c r="G36" s="21">
+        <v>1</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="L36" s="15" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>103</v>
+        <v>339</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G37" s="23"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>339</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>340</v>
+      <c r="E38" s="3"/>
+      <c r="G38" s="21">
+        <v>2</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="3" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E39" s="3"/>
+      <c r="G39" s="19">
+        <v>3</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="3" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>112</v>
+        <v>329</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>330</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G40" s="9">
+        <v>4</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>329</v>
+        <v>94</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>330</v>
+        <v>99</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>301</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="A43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3" t="s">
-        <v>387</v>
-      </c>
+      <c r="E43" s="3"/>
       <c r="G43" s="6" t="s">
         <v>168</v>
       </c>
@@ -3376,17 +3472,6 @@
       </c>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
       <c r="G44" s="7" t="s">
         <v>123</v>
       </c>
@@ -3906,7 +3991,7 @@
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G62" s="18">
         <v>7</v>
@@ -5166,36 +5251,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="33" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="33" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5203,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -5220,7 +5305,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5237,7 +5322,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5254,7 +5339,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -5271,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -5288,7 +5373,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C8">
         <v>2</v>

</xml_diff>